<commit_message>
update ai confidence in food prediction feature and update in third feature
</commit_message>
<xml_diff>
--- a/application/Documentation/Document.xlsx
+++ b/application/Documentation/Document.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Icoach-app\application\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFB9FB1-7063-49EA-A4CD-2079AF1E9E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271F99EA-483A-4F22-AAB7-EAF134B724B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="232">
   <si>
     <t>Exercise Name</t>
   </si>
@@ -511,13 +511,223 @@
   </si>
   <si>
     <t>Great!</t>
+  </si>
+  <si>
+    <t>Lateral Raises</t>
+  </si>
+  <si>
+    <t>Arms or shoulders cut off</t>
+  </si>
+  <si>
+    <t>Step back for arm clearance</t>
+  </si>
+  <si>
+    <t>"Step back"</t>
+  </si>
+  <si>
+    <t>CMD_RAISE_ARMS</t>
+  </si>
+  <si>
+    <t>Arms resting at sides</t>
+  </si>
+  <si>
+    <t>Raise arms sideways</t>
+  </si>
+  <si>
+    <t>"Arms up"</t>
+  </si>
+  <si>
+    <t>STRAIGHTEN_ARMS</t>
+  </si>
+  <si>
+    <t>Elbow angle &lt; 155°</t>
+  </si>
+  <si>
+    <t>"Straighten arms"</t>
+  </si>
+  <si>
+    <t>ERR_TOO_HIGH</t>
+  </si>
+  <si>
+    <t>Arms above shoulder level</t>
+  </si>
+  <si>
+    <t>Don't go above shoulders</t>
+  </si>
+  <si>
+    <t>"Too high"</t>
+  </si>
+  <si>
+    <t>PERFECT</t>
+  </si>
+  <si>
+    <t>Arms at 85-90°</t>
+  </si>
+  <si>
+    <t>Perfect Level</t>
+  </si>
+  <si>
+    <t>"Hold"</t>
+  </si>
+  <si>
+    <t>Controlled movement</t>
+  </si>
+  <si>
+    <t>Excellent Rep!</t>
+  </si>
+  <si>
+    <t>"Good"</t>
+  </si>
+  <si>
+    <t>Front Raises</t>
+  </si>
+  <si>
+    <t>Arms/torso not visible</t>
+  </si>
+  <si>
+    <t>Adjust position, show arms</t>
+  </si>
+  <si>
+    <t>"Show arms"</t>
+  </si>
+  <si>
+    <t>CMD_RAISE_FRONT</t>
+  </si>
+  <si>
+    <t>Arms at start pos</t>
+  </si>
+  <si>
+    <t>Raise arms in front</t>
+  </si>
+  <si>
+    <t>"Raise front"</t>
+  </si>
+  <si>
+    <t>RAISE_YOUR_ARM</t>
+  </si>
+  <si>
+    <t>Arms &lt; 85°</t>
+  </si>
+  <si>
+    <t>Raise higher to chest level</t>
+  </si>
+  <si>
+    <t>"Higher"</t>
+  </si>
+  <si>
+    <t>ERR_SWINGING</t>
+  </si>
+  <si>
+    <t>Momentum usage</t>
+  </si>
+  <si>
+    <t>Keep your torso still</t>
+  </si>
+  <si>
+    <t>"Don't swing"</t>
+  </si>
+  <si>
+    <t>GOOD_REP</t>
+  </si>
+  <si>
+    <t>Peak angle reached</t>
+  </si>
+  <si>
+    <t>Good Control</t>
+  </si>
+  <si>
+    <t>"Nice"</t>
+  </si>
+  <si>
+    <t>Rep counted</t>
+  </si>
+  <si>
+    <t>Nice Work!</t>
+  </si>
+  <si>
+    <t>Overhead Press</t>
+  </si>
+  <si>
+    <t>Stand tall, weights at shoulders</t>
+  </si>
+  <si>
+    <t>"Stand tall"</t>
+  </si>
+  <si>
+    <t>ERR_CAMERA_VIEW</t>
+  </si>
+  <si>
+    <t>Hands overhead &lt; 0.5 vis</t>
+  </si>
+  <si>
+    <t>Arms must be visible overhead</t>
+  </si>
+  <si>
+    <t>"Fix camera"</t>
+  </si>
+  <si>
+    <t>ERR_ARCHED_BACK</t>
+  </si>
+  <si>
+    <t>Shoulder-Hip dist &gt; 0.15</t>
+  </si>
+  <si>
+    <t>Keep core tight, don't lean back</t>
+  </si>
+  <si>
+    <t>"Don't lean"</t>
+  </si>
+  <si>
+    <t>ERR_LOW_ARMS</t>
+  </si>
+  <si>
+    <t>Elbow Y &gt; Shoulder Y + 0.1</t>
+  </si>
+  <si>
+    <t>Don't drop elbows too low</t>
+  </si>
+  <si>
+    <t>"Elbows up"</t>
+  </si>
+  <si>
+    <t>PUSH_UP</t>
+  </si>
+  <si>
+    <t>Elbow angle &lt; 75°</t>
+  </si>
+  <si>
+    <t>Press overhead</t>
+  </si>
+  <si>
+    <t>"Press up"</t>
+  </si>
+  <si>
+    <t>LOWER_SLOWLY</t>
+  </si>
+  <si>
+    <t>Elbow angle &gt; 165°</t>
+  </si>
+  <si>
+    <t>Lower firmly to shoulders</t>
+  </si>
+  <si>
+    <t>"Lower"</t>
+  </si>
+  <si>
+    <t>Returned to start</t>
+  </si>
+  <si>
+    <t>Great lift!</t>
+  </si>
+  <si>
+    <t>"Great"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -530,6 +740,13 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -539,7 +756,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -547,13 +764,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,14 +946,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4AA153B-FF24-47A9-930C-B391914616BC}" name="Table1" displayName="Table1" ref="A1:E48" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:E48" xr:uid="{C4AA153B-FF24-47A9-930C-B391914616BC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4AA153B-FF24-47A9-930C-B391914616BC}" name="Table1" displayName="Table1" ref="A1:E67" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E67" xr:uid="{C4AA153B-FF24-47A9-930C-B391914616BC}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D1458035-9B3B-4CB2-8959-57596F805A93}" name="Exercise Name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F850DA0A-9A5A-448A-B989-249F2645FC8B}" name="Feedback Code (Python)" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{88EA5755-7254-497D-AFAA-61C55B3D2DC5}" name="Logic / Condition (Trigger)" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A900BBEC-8CF7-456E-A175-1B5323C50376}" name="UI Message (Text to Display)" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{FED98BA3-7FEB-44DC-A961-FBCB52C862FC}" name="Audio File Name (Suggested)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{D1458035-9B3B-4CB2-8959-57596F805A93}" name="Exercise Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{F850DA0A-9A5A-448A-B989-249F2645FC8B}" name="Feedback Code (Python)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{88EA5755-7254-497D-AFAA-61C55B3D2DC5}" name="Logic / Condition (Trigger)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A900BBEC-8CF7-456E-A175-1B5323C50376}" name="UI Message (Text to Display)" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{FED98BA3-7FEB-44DC-A961-FBCB52C862FC}" name="Audio File Name (Suggested)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -913,10 +1160,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1727,7 +1974,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>136</v>
       </c>
@@ -1742,6 +1989,329 @@
       </c>
       <c r="E48" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>